<commit_message>
sincronizando upload e download para usarem a mesma planilha
</commit_message>
<xml_diff>
--- a/public/template-usuarios.xlsx
+++ b/public/template-usuarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Main\Projects\house\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82C872-AC26-4040-98C1-C5DCA0CA9FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DC826-390B-41FA-853D-198C10954706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="590" yWindow="110" windowWidth="18610" windowHeight="9970" xr2:uid="{06EAEF6F-C33D-4D4D-A0EB-4A70EF3A93C8}"/>
+    <workbookView xWindow="590" yWindow="830" windowWidth="18610" windowHeight="9970" xr2:uid="{06EAEF6F-C33D-4D4D-A0EB-4A70EF3A93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>cpf</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>cargo</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -78,12 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,34 +400,33 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -436,7 +434,6 @@
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -444,7 +441,6 @@
     </row>
     <row r="4" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>